<commit_message>
Re-edit to remove Bed No. for MNH Pharmacy & Update Ward No
</commit_message>
<xml_diff>
--- a/IS447/System/Data/Pharmacy Dept/GEH TTO Data/GEH TTO TAT 2021 Aug.xlsx
+++ b/IS447/System/Data/Pharmacy Dept/GEH TTO Data/GEH TTO TAT 2021 Aug.xlsx
@@ -1,33 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\3. Operational\3c. TTO Statistics\TTO TAT DATA\Raw Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sherminliam/Documents/School Work/IS447/IS447---Smart-Healthcare/IS447/System/Data/Pharmacy Dept/GEH TTO Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808722E4-2BBC-1E43-A6DC-A028620DC1C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9380"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="19200" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Z$390</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$W$345</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2735" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2733" uniqueCount="105">
   <si>
     <t>No</t>
   </si>
@@ -290,13 +301,7 @@
     <t>Ai Ling Stephanie Poh</t>
   </si>
   <si>
-    <t>Icu 18</t>
-  </si>
-  <si>
     <t>Jia yun</t>
-  </si>
-  <si>
-    <t>ICU3</t>
   </si>
   <si>
     <t>Shahida</t>
@@ -353,7 +358,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -727,29 +732,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z390"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.6328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.90625" style="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.1796875" customWidth="1"/>
-    <col min="19" max="19" width="14.81640625" customWidth="1"/>
-    <col min="20" max="20" width="18.54296875" customWidth="1"/>
-    <col min="26" max="26" width="8.90625" style="15"/>
+    <col min="11" max="11" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.83203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.1640625" customWidth="1"/>
+    <col min="19" max="19" width="14.83203125" customWidth="1"/>
+    <col min="20" max="20" width="18.5" customWidth="1"/>
+    <col min="26" max="26" width="8.83203125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -823,7 +828,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="19">
         <v>44409</v>
       </c>
@@ -885,7 +890,7 @@
         <v>14.583333333333332</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="19">
         <v>44409</v>
       </c>
@@ -943,11 +948,11 @@
       <c r="X3" s="10"/>
       <c r="Y3" s="14"/>
       <c r="Z3" s="15">
-        <f t="shared" ref="Z2:Z18" si="0">N3*1400</f>
+        <f t="shared" ref="Z3:Z18" si="0">N3*1400</f>
         <v>55.416666666666664</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="19">
         <v>44409</v>
       </c>
@@ -997,7 +1002,7 @@
         <v>543.47222222222229</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="19">
         <v>44409</v>
       </c>
@@ -1059,7 +1064,7 @@
         <v>29.166666666666664</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="19">
         <v>44409</v>
       </c>
@@ -1121,7 +1126,7 @@
         <v>3.8888888888888888</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="19">
         <v>44409</v>
       </c>
@@ -1183,7 +1188,7 @@
         <v>15.555555555555555</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="19">
         <v>44410</v>
       </c>
@@ -1245,7 +1250,7 @@
         <v>145.83333333333334</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="19">
         <v>44410</v>
       </c>
@@ -1307,7 +1312,7 @@
         <v>37.916666666666671</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="19">
         <v>44410</v>
       </c>
@@ -1369,7 +1374,7 @@
         <v>38.888888888888886</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="19">
         <v>44410</v>
       </c>
@@ -1428,7 +1433,7 @@
         <v>90.416666666666671</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="19">
         <v>44410</v>
       </c>
@@ -1490,7 +1495,7 @@
         <v>21.388888888888889</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="19">
         <v>44411</v>
       </c>
@@ -1552,7 +1557,7 @@
         <v>25.277777777777779</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="19">
         <v>44411</v>
       </c>
@@ -1611,7 +1616,7 @@
         <v>18.472222222222221</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="19">
         <v>44411</v>
       </c>
@@ -1673,7 +1678,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="19">
         <v>44411</v>
       </c>
@@ -1735,7 +1740,7 @@
         <v>31.111111111111111</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="19">
         <v>44411</v>
       </c>
@@ -1797,7 +1802,7 @@
         <v>52.5</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="19">
         <v>44411</v>
       </c>
@@ -1859,7 +1864,7 @@
         <v>48.611111111111114</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="19">
         <v>44411</v>
       </c>
@@ -1921,7 +1926,7 @@
         <v>30.138888888888893</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="19">
         <v>44411</v>
       </c>
@@ -1986,7 +1991,7 @@
         <v>469.58333333333337</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="19">
         <v>44411</v>
       </c>
@@ -2039,7 +2044,7 @@
         <v>587.22222222222229</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="19">
         <v>44411</v>
       </c>
@@ -2092,7 +2097,7 @@
         <v>608.61111111111109</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="19">
         <v>44411</v>
       </c>
@@ -2154,7 +2159,7 @@
         <v>24.305555555555557</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24" s="19">
         <v>44411</v>
       </c>
@@ -2216,7 +2221,7 @@
         <v>54.444444444444443</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25" s="19">
         <v>44411</v>
       </c>
@@ -2278,7 +2283,7 @@
         <v>26.25</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26" s="19">
         <v>44411</v>
       </c>
@@ -2337,7 +2342,7 @@
         <v>19.444444444444443</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27" s="19">
         <v>44411</v>
       </c>
@@ -2384,7 +2389,7 @@
         <v>960.55555555555543</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28" s="19">
         <v>44411</v>
       </c>
@@ -2437,7 +2442,7 @@
         <v>994.58333333333337</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" s="19">
         <v>44412</v>
       </c>
@@ -2502,7 +2507,7 @@
         <v>113.75</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A30" s="19">
         <v>44412</v>
       </c>
@@ -2564,7 +2569,7 @@
         <v>33.055555555555557</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A31" s="19">
         <v>44412</v>
       </c>
@@ -2626,7 +2631,7 @@
         <v>30.138888888888893</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A32" s="19">
         <v>44412</v>
       </c>
@@ -2685,7 +2690,7 @@
         <v>42.777777777777779</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A33" s="19">
         <v>44412</v>
       </c>
@@ -2747,7 +2752,7 @@
         <v>34.027777777777779</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A34" s="19">
         <v>44412</v>
       </c>
@@ -2806,7 +2811,7 @@
         <v>49.583333333333329</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A35" s="19">
         <v>44412</v>
       </c>
@@ -2868,7 +2873,7 @@
         <v>15.555555555555555</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A36" s="19">
         <v>44412</v>
       </c>
@@ -2930,7 +2935,7 @@
         <v>19.444444444444443</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A37" s="19">
         <v>44412</v>
       </c>
@@ -2995,7 +3000,7 @@
         <v>36.944444444444443</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A38" s="19">
         <v>44412</v>
       </c>
@@ -3057,7 +3062,7 @@
         <v>68.055555555555557</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A39" s="19">
         <v>44412</v>
       </c>
@@ -3119,7 +3124,7 @@
         <v>0.97222222222222221</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A40" s="19">
         <v>44412</v>
       </c>
@@ -3181,7 +3186,7 @@
         <v>13.611111111111111</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A41" s="19">
         <v>44412</v>
       </c>
@@ -3243,7 +3248,7 @@
         <v>13.611111111111111</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A42" s="19">
         <v>44412</v>
       </c>
@@ -3290,7 +3295,7 @@
         <v>1009.1666666666666</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A43" s="19">
         <v>44413</v>
       </c>
@@ -3352,7 +3357,7 @@
         <v>19.444444444444443</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A44" s="19">
         <v>44413</v>
       </c>
@@ -3417,7 +3422,7 @@
         <v>10.694444444444445</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45" s="19">
         <v>44413</v>
       </c>
@@ -3470,7 +3475,7 @@
         <v>516.25</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A46" s="19">
         <v>44413</v>
       </c>
@@ -3532,7 +3537,7 @@
         <v>33.055555555555557</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A47" s="19">
         <v>44413</v>
       </c>
@@ -3585,7 +3590,7 @@
         <v>530.83333333333326</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A48" s="19">
         <v>44413</v>
       </c>
@@ -3647,7 +3652,7 @@
         <v>12.638888888888889</v>
       </c>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A49" s="19">
         <v>44413</v>
       </c>
@@ -3694,7 +3699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A50" s="19">
         <v>44413</v>
       </c>
@@ -3750,7 +3755,7 @@
         <v>622.22222222222217</v>
       </c>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A51" s="19">
         <v>44413</v>
       </c>
@@ -3812,7 +3817,7 @@
         <v>64.166666666666671</v>
       </c>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A52" s="19">
         <v>44413</v>
       </c>
@@ -3859,7 +3864,7 @@
         <v>637.77777777777771</v>
       </c>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A53" s="19">
         <v>44413</v>
       </c>
@@ -3915,7 +3920,7 @@
         <v>687.36111111111109</v>
       </c>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A54" s="19">
         <v>44413</v>
       </c>
@@ -3965,7 +3970,7 @@
         <v>687.36111111111109</v>
       </c>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A55" s="19">
         <v>44413</v>
       </c>
@@ -4030,7 +4035,7 @@
         <v>14.583333333333332</v>
       </c>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A56" s="19">
         <v>44413</v>
       </c>
@@ -4092,7 +4097,7 @@
         <v>62.222222222222221</v>
       </c>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A57" s="19">
         <v>44413</v>
       </c>
@@ -4139,7 +4144,7 @@
         <v>958.61111111111109</v>
       </c>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A58" s="19">
         <v>44413</v>
       </c>
@@ -4201,7 +4206,7 @@
         <v>240.13888888888886</v>
       </c>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A59" s="19">
         <v>44414</v>
       </c>
@@ -4257,7 +4262,7 @@
         <v>505.55555555555554</v>
       </c>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A60" s="19">
         <v>44414</v>
       </c>
@@ -4310,7 +4315,7 @@
         <v>551.25</v>
       </c>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A61" s="19">
         <v>44414</v>
       </c>
@@ -4363,7 +4368,7 @@
         <v>553.19444444444446</v>
       </c>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A62" s="19">
         <v>44414</v>
       </c>
@@ -4416,7 +4421,7 @@
         <v>557.08333333333337</v>
       </c>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A63" s="19">
         <v>44414</v>
       </c>
@@ -4478,7 +4483,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A64" s="19">
         <v>44414</v>
       </c>
@@ -4531,7 +4536,7 @@
         <v>563.8888888888888</v>
       </c>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A65" s="19">
         <v>44414</v>
       </c>
@@ -4593,7 +4598,7 @@
         <v>20.416666666666664</v>
       </c>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A66" s="19">
         <v>44414</v>
       </c>
@@ -4655,7 +4660,7 @@
         <v>36.944444444444443</v>
       </c>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A67" s="19">
         <v>44414</v>
       </c>
@@ -4717,7 +4722,7 @@
         <v>25.277777777777779</v>
       </c>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A68" s="19">
         <v>44414</v>
       </c>
@@ -4779,7 +4784,7 @@
         <v>23.333333333333332</v>
       </c>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A69" s="19">
         <v>44414</v>
       </c>
@@ -4841,7 +4846,7 @@
         <v>24.305555555555557</v>
       </c>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A70" s="19">
         <v>44414</v>
       </c>
@@ -4888,7 +4893,7 @@
         <v>832.22222222222217</v>
       </c>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A71" s="19">
         <v>44414</v>
       </c>
@@ -4950,7 +4955,7 @@
         <v>43.75</v>
       </c>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A72" s="19">
         <v>44414</v>
       </c>
@@ -5012,7 +5017,7 @@
         <v>45.69444444444445</v>
       </c>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A73" s="19">
         <v>44414</v>
       </c>
@@ -5074,7 +5079,7 @@
         <v>29.166666666666664</v>
       </c>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A74" s="19">
         <v>44415</v>
       </c>
@@ -5136,7 +5141,7 @@
         <v>32.083333333333336</v>
       </c>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A75" s="19">
         <v>44415</v>
       </c>
@@ -5198,7 +5203,7 @@
         <v>50.555555555555557</v>
       </c>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A76" s="19">
         <v>44415</v>
       </c>
@@ -5260,7 +5265,7 @@
         <v>44.722222222222229</v>
       </c>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A77" s="19">
         <v>44415</v>
       </c>
@@ -5322,7 +5327,7 @@
         <v>47.638888888888886</v>
       </c>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A78" s="19">
         <v>44415</v>
       </c>
@@ -5384,7 +5389,7 @@
         <v>38.888888888888886</v>
       </c>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A79" s="19">
         <v>44415</v>
       </c>
@@ -5443,7 +5448,7 @@
         <v>41.805555555555557</v>
       </c>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A80" s="19">
         <v>44415</v>
       </c>
@@ -5505,7 +5510,7 @@
         <v>52.5</v>
       </c>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A81" s="19">
         <v>44416</v>
       </c>
@@ -5567,7 +5572,7 @@
         <v>29.166666666666664</v>
       </c>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A82" s="19">
         <v>44416</v>
       </c>
@@ -5623,7 +5628,7 @@
         <v>47.638888888888886</v>
       </c>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A83" s="19">
         <v>44416</v>
       </c>
@@ -5685,7 +5690,7 @@
         <v>19.444444444444443</v>
       </c>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A84" s="19">
         <v>44416</v>
       </c>
@@ -5741,7 +5746,7 @@
         <v>14.583333333333332</v>
       </c>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A85" s="19">
         <v>44418</v>
       </c>
@@ -5803,7 +5808,7 @@
         <v>28.194444444444446</v>
       </c>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A86" s="19">
         <v>44418</v>
       </c>
@@ -5850,7 +5855,7 @@
         <v>499.72222222222223</v>
       </c>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A87" s="19">
         <v>44418</v>
       </c>
@@ -5912,7 +5917,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A88" s="19">
         <v>44418</v>
       </c>
@@ -5974,7 +5979,7 @@
         <v>18.472222222222221</v>
       </c>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A89" s="19">
         <v>44418</v>
       </c>
@@ -6021,7 +6026,7 @@
         <v>600.83333333333337</v>
       </c>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A90" s="19">
         <v>44418</v>
       </c>
@@ -6083,7 +6088,7 @@
         <v>14.583333333333332</v>
       </c>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A91" s="19">
         <v>44418</v>
       </c>
@@ -6145,7 +6150,7 @@
         <v>58.333333333333329</v>
       </c>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A92" s="19">
         <v>44418</v>
       </c>
@@ -6210,7 +6215,7 @@
         <v>12.638888888888889</v>
       </c>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A93" s="19">
         <v>44418</v>
       </c>
@@ -6272,7 +6277,7 @@
         <v>24.305555555555557</v>
       </c>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A94" s="19">
         <v>44418</v>
       </c>
@@ -6334,7 +6339,7 @@
         <v>409.3055555555556</v>
       </c>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A95" s="19">
         <v>44419</v>
       </c>
@@ -6399,7 +6404,7 @@
         <v>182.7777777777778</v>
       </c>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A96" s="19">
         <v>44419</v>
       </c>
@@ -6461,7 +6466,7 @@
         <v>42.777777777777779</v>
       </c>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A97" s="19">
         <v>44419</v>
       </c>
@@ -6526,7 +6531,7 @@
         <v>62.222222222222221</v>
       </c>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A98" s="19">
         <v>44419</v>
       </c>
@@ -6579,7 +6584,7 @@
         <v>566.80555555555554</v>
       </c>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A99" s="19">
         <v>44419</v>
       </c>
@@ -6626,7 +6631,7 @@
         <v>581.38888888888891</v>
       </c>
     </row>
-    <row r="100" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A100" s="19">
         <v>44419</v>
       </c>
@@ -6688,7 +6693,7 @@
         <v>50.555555555555557</v>
       </c>
     </row>
-    <row r="101" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A101" s="19">
         <v>44419</v>
       </c>
@@ -6750,7 +6755,7 @@
         <v>50.555555555555557</v>
       </c>
     </row>
-    <row r="102" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A102" s="19">
         <v>44419</v>
       </c>
@@ -6812,7 +6817,7 @@
         <v>64.166666666666671</v>
       </c>
     </row>
-    <row r="103" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A103" s="19">
         <v>44419</v>
       </c>
@@ -6874,7 +6879,7 @@
         <v>48.611111111111114</v>
       </c>
     </row>
-    <row r="104" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A104" s="19">
         <v>44419</v>
       </c>
@@ -6921,7 +6926,7 @@
         <v>836.11111111111109</v>
       </c>
     </row>
-    <row r="105" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A105" s="19">
         <v>44419</v>
       </c>
@@ -6983,7 +6988,7 @@
         <v>43.75</v>
       </c>
     </row>
-    <row r="106" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A106" s="19">
         <v>44420</v>
       </c>
@@ -7030,7 +7035,7 @@
         <v>543.47222222222229</v>
       </c>
     </row>
-    <row r="107" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A107" s="19">
         <v>44420</v>
       </c>
@@ -7092,7 +7097,7 @@
         <v>32.083333333333336</v>
       </c>
     </row>
-    <row r="108" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A108" s="19">
         <v>44420</v>
       </c>
@@ -7151,7 +7156,7 @@
         <v>29.166666666666664</v>
       </c>
     </row>
-    <row r="109" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A109" s="19">
         <v>44420</v>
       </c>
@@ -7213,7 +7218,7 @@
         <v>87.5</v>
       </c>
     </row>
-    <row r="110" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A110" s="19">
         <v>44420</v>
       </c>
@@ -7275,7 +7280,7 @@
         <v>60.277777777777786</v>
       </c>
     </row>
-    <row r="111" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A111" s="19">
         <v>44420</v>
       </c>
@@ -7334,7 +7339,7 @@
         <v>29.166666666666664</v>
       </c>
     </row>
-    <row r="112" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A112" s="19">
         <v>44421</v>
       </c>
@@ -7396,7 +7401,7 @@
         <v>82.6388888888889</v>
       </c>
     </row>
-    <row r="113" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A113" s="19">
         <v>44421</v>
       </c>
@@ -7458,7 +7463,7 @@
         <v>77.777777777777771</v>
       </c>
     </row>
-    <row r="114" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A114" s="19">
         <v>44421</v>
       </c>
@@ -7523,7 +7528,7 @@
         <v>57.361111111111114</v>
       </c>
     </row>
-    <row r="115" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A115" s="19">
         <v>44421</v>
       </c>
@@ -7585,7 +7590,7 @@
         <v>78.75</v>
       </c>
     </row>
-    <row r="116" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A116" s="19">
         <v>44421</v>
       </c>
@@ -7647,7 +7652,7 @@
         <v>92.361111111111114</v>
       </c>
     </row>
-    <row r="117" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A117" s="19">
         <v>44421</v>
       </c>
@@ -7712,7 +7717,7 @@
         <v>48.611111111111114</v>
       </c>
     </row>
-    <row r="118" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A118" s="19">
         <v>44421</v>
       </c>
@@ -7774,7 +7779,7 @@
         <v>68.055555555555557</v>
       </c>
     </row>
-    <row r="119" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A119" s="19">
         <v>44421</v>
       </c>
@@ -7833,7 +7838,7 @@
         <v>30.138888888888893</v>
       </c>
     </row>
-    <row r="120" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A120" s="19">
         <v>44421</v>
       </c>
@@ -7895,7 +7900,7 @@
         <v>26.25</v>
       </c>
     </row>
-    <row r="121" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A121" s="19">
         <v>44421</v>
       </c>
@@ -7954,7 +7959,7 @@
         <v>13.611111111111111</v>
       </c>
     </row>
-    <row r="122" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A122" s="19">
         <v>44421</v>
       </c>
@@ -8016,7 +8021,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="123" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A123" s="19">
         <v>44422</v>
       </c>
@@ -8063,7 +8068,7 @@
         <v>511.38888888888891</v>
       </c>
     </row>
-    <row r="124" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A124" s="19">
         <v>44422</v>
       </c>
@@ -8128,7 +8133,7 @@
         <v>79.722222222222214</v>
       </c>
     </row>
-    <row r="125" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A125" s="19">
         <v>44422</v>
       </c>
@@ -8184,7 +8189,7 @@
         <v>513.33333333333337</v>
       </c>
     </row>
-    <row r="126" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A126" s="19">
         <v>44422</v>
       </c>
@@ -8246,7 +8251,7 @@
         <v>26.25</v>
       </c>
     </row>
-    <row r="127" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A127" s="19">
         <v>44422</v>
       </c>
@@ -8302,7 +8307,7 @@
         <v>555.13888888888891</v>
       </c>
     </row>
-    <row r="128" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A128" s="19">
         <v>44422</v>
       </c>
@@ -8364,7 +8369,7 @@
         <v>24.305555555555557</v>
       </c>
     </row>
-    <row r="129" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A129" s="19">
         <v>44422</v>
       </c>
@@ -8423,7 +8428,7 @@
         <v>35.972222222222229</v>
       </c>
     </row>
-    <row r="130" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A130" s="19">
         <v>44422</v>
       </c>
@@ -8482,7 +8487,7 @@
         <v>34.027777777777779</v>
       </c>
     </row>
-    <row r="131" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A131" s="19">
         <v>44422</v>
       </c>
@@ -8544,7 +8549,7 @@
         <v>55.416666666666664</v>
       </c>
     </row>
-    <row r="132" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A132" s="19">
         <v>44422</v>
       </c>
@@ -8609,7 +8614,7 @@
         <v>48.611111111111114</v>
       </c>
     </row>
-    <row r="133" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A133" s="19">
         <v>44422</v>
       </c>
@@ -8671,7 +8676,7 @@
         <v>29.166666666666664</v>
       </c>
     </row>
-    <row r="134" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A134" s="19">
         <v>44422</v>
       </c>
@@ -8718,7 +8723,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="135" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A135" s="19">
         <v>44422</v>
       </c>
@@ -8771,7 +8776,7 @@
         <v>695.1388888888888</v>
       </c>
     </row>
-    <row r="136" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A136" s="19">
         <v>44422</v>
       </c>
@@ -8833,7 +8838,7 @@
         <v>30.138888888888893</v>
       </c>
     </row>
-    <row r="137" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A137" s="19">
         <v>44422</v>
       </c>
@@ -8895,7 +8900,7 @@
         <v>48.611111111111114</v>
       </c>
     </row>
-    <row r="138" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A138" s="19">
         <v>44422</v>
       </c>
@@ -8957,7 +8962,7 @@
         <v>40.833333333333329</v>
       </c>
     </row>
-    <row r="139" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A139" s="19">
         <v>44422</v>
       </c>
@@ -9019,7 +9024,7 @@
         <v>24.305555555555557</v>
       </c>
     </row>
-    <row r="140" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A140" s="19">
         <v>44423</v>
       </c>
@@ -9081,7 +9086,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="141" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A141" s="19">
         <v>44423</v>
       </c>
@@ -9143,7 +9148,7 @@
         <v>40.833333333333329</v>
       </c>
     </row>
-    <row r="142" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A142" s="19">
         <v>44423</v>
       </c>
@@ -9202,7 +9207,7 @@
         <v>19.444444444444443</v>
       </c>
     </row>
-    <row r="143" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A143" s="19">
         <v>44423</v>
       </c>
@@ -9255,7 +9260,7 @@
         <v>1.9444444444444444</v>
       </c>
     </row>
-    <row r="144" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A144" s="19">
         <v>44423</v>
       </c>
@@ -9308,7 +9313,7 @@
         <v>654.30555555555554</v>
       </c>
     </row>
-    <row r="145" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A145" s="19">
         <v>44423</v>
       </c>
@@ -9367,7 +9372,7 @@
         <v>74.861111111111114</v>
       </c>
     </row>
-    <row r="146" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A146" s="19">
         <v>44423</v>
       </c>
@@ -9429,7 +9434,7 @@
         <v>65.138888888888886</v>
       </c>
     </row>
-    <row r="147" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A147" s="19">
         <v>44423</v>
       </c>
@@ -9491,7 +9496,7 @@
         <v>55.416666666666664</v>
       </c>
     </row>
-    <row r="148" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A148" s="19">
         <v>44423</v>
       </c>
@@ -9538,7 +9543,7 @@
         <v>768.05555555555543</v>
       </c>
     </row>
-    <row r="149" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A149" s="19">
         <v>44424</v>
       </c>
@@ -9600,7 +9605,7 @@
         <v>36.944444444444443</v>
       </c>
     </row>
-    <row r="150" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A150" s="19">
         <v>44424</v>
       </c>
@@ -9662,7 +9667,7 @@
         <v>39.861111111111107</v>
       </c>
     </row>
-    <row r="151" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A151" s="19">
         <v>44424</v>
       </c>
@@ -9724,7 +9729,7 @@
         <v>25.277777777777779</v>
       </c>
     </row>
-    <row r="152" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A152" s="19">
         <v>44424</v>
       </c>
@@ -9783,7 +9788,7 @@
         <v>102.08333333333334</v>
       </c>
     </row>
-    <row r="153" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A153" s="19">
         <v>44424</v>
       </c>
@@ -9845,7 +9850,7 @@
         <v>24.305555555555557</v>
       </c>
     </row>
-    <row r="154" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A154" s="19">
         <v>44424</v>
       </c>
@@ -9907,7 +9912,7 @@
         <v>45.69444444444445</v>
       </c>
     </row>
-    <row r="155" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A155" s="19">
         <v>44424</v>
       </c>
@@ -9969,7 +9974,7 @@
         <v>24.305555555555557</v>
       </c>
     </row>
-    <row r="156" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A156" s="19">
         <v>44424</v>
       </c>
@@ -10031,7 +10036,7 @@
         <v>66.111111111111114</v>
       </c>
     </row>
-    <row r="157" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A157" s="19">
         <v>44424</v>
       </c>
@@ -10093,7 +10098,7 @@
         <v>43.75</v>
       </c>
     </row>
-    <row r="158" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A158" s="19">
         <v>44424</v>
       </c>
@@ -10140,7 +10145,7 @@
         <v>686.38888888888891</v>
       </c>
     </row>
-    <row r="159" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A159" s="19">
         <v>44424</v>
       </c>
@@ -10202,7 +10207,7 @@
         <v>39.861111111111107</v>
       </c>
     </row>
-    <row r="160" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A160" s="19">
         <v>44424</v>
       </c>
@@ -10261,7 +10266,7 @@
         <v>37.916666666666671</v>
       </c>
     </row>
-    <row r="161" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A161" s="19">
         <v>44424</v>
       </c>
@@ -10323,7 +10328,7 @@
         <v>4.8611111111111107</v>
       </c>
     </row>
-    <row r="162" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A162" s="19">
         <v>44425</v>
       </c>
@@ -10385,7 +10390,7 @@
         <v>98.194444444444443</v>
       </c>
     </row>
-    <row r="163" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A163" s="19">
         <v>44425</v>
       </c>
@@ -10447,7 +10452,7 @@
         <v>189.58333333333331</v>
       </c>
     </row>
-    <row r="164" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A164" s="19">
         <v>44425</v>
       </c>
@@ -10509,7 +10514,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="165" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A165" s="19">
         <v>44425</v>
       </c>
@@ -10574,7 +10579,7 @@
         <v>76.805555555555557</v>
       </c>
     </row>
-    <row r="166" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A166" s="19">
         <v>44425</v>
       </c>
@@ -10633,7 +10638,7 @@
         <v>105.97222222222221</v>
       </c>
     </row>
-    <row r="167" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A167" s="19">
         <v>44425</v>
       </c>
@@ -10692,7 +10697,7 @@
         <v>24.305555555555557</v>
       </c>
     </row>
-    <row r="168" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A168" s="19">
         <v>44425</v>
       </c>
@@ -10751,7 +10756,7 @@
         <v>12.638888888888889</v>
       </c>
     </row>
-    <row r="169" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A169" s="19">
         <v>44425</v>
       </c>
@@ -10813,7 +10818,7 @@
         <v>37.916666666666671</v>
       </c>
     </row>
-    <row r="170" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A170" s="19">
         <v>44425</v>
       </c>
@@ -10875,7 +10880,7 @@
         <v>78.75</v>
       </c>
     </row>
-    <row r="171" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A171" s="19">
         <v>44425</v>
       </c>
@@ -10937,7 +10942,7 @@
         <v>33.055555555555557</v>
       </c>
     </row>
-    <row r="172" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A172" s="19">
         <v>44425</v>
       </c>
@@ -10999,7 +11004,7 @@
         <v>33.055555555555557</v>
       </c>
     </row>
-    <row r="173" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A173" s="19">
         <v>44426</v>
       </c>
@@ -11061,7 +11066,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="174" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A174" s="19">
         <v>44426</v>
       </c>
@@ -11123,7 +11128,7 @@
         <v>53.472222222222214</v>
       </c>
     </row>
-    <row r="175" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A175" s="19">
         <v>44426</v>
       </c>
@@ -11185,7 +11190,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="176" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A176" s="19">
         <v>44426</v>
       </c>
@@ -11247,7 +11252,7 @@
         <v>126.38888888888889</v>
       </c>
     </row>
-    <row r="177" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A177" s="19">
         <v>44426</v>
       </c>
@@ -11309,7 +11314,7 @@
         <v>55.416666666666664</v>
       </c>
     </row>
-    <row r="178" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A178" s="19">
         <v>44426</v>
       </c>
@@ -11371,7 +11376,7 @@
         <v>24.305555555555557</v>
       </c>
     </row>
-    <row r="179" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A179" s="19">
         <v>44426</v>
       </c>
@@ -11436,7 +11441,7 @@
         <v>361.66666666666669</v>
       </c>
     </row>
-    <row r="180" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A180" s="19">
         <v>44426</v>
       </c>
@@ -11498,7 +11503,7 @@
         <v>79.722222222222214</v>
       </c>
     </row>
-    <row r="181" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A181" s="19">
         <v>44426</v>
       </c>
@@ -11557,7 +11562,7 @@
         <v>47.638888888888886</v>
       </c>
     </row>
-    <row r="182" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A182" s="19">
         <v>44426</v>
       </c>
@@ -11619,7 +11624,7 @@
         <v>53.472222222222214</v>
       </c>
     </row>
-    <row r="183" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A183" s="19">
         <v>44427</v>
       </c>
@@ -11681,7 +11686,7 @@
         <v>29.166666666666664</v>
       </c>
     </row>
-    <row r="184" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A184" s="19">
         <v>44427</v>
       </c>
@@ -11740,7 +11745,7 @@
         <v>34.027777777777779</v>
       </c>
     </row>
-    <row r="185" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A185" s="19">
         <v>44427</v>
       </c>
@@ -11802,7 +11807,7 @@
         <v>77.777777777777771</v>
       </c>
     </row>
-    <row r="186" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A186" s="19">
         <v>44427</v>
       </c>
@@ -11864,7 +11869,7 @@
         <v>90.416666666666671</v>
       </c>
     </row>
-    <row r="187" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A187" s="19">
         <v>44427</v>
       </c>
@@ -11917,7 +11922,7 @@
         <v>564.86111111111109</v>
       </c>
     </row>
-    <row r="188" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A188" s="19">
         <v>44427</v>
       </c>
@@ -11979,7 +11984,7 @@
         <v>33.055555555555557</v>
       </c>
     </row>
-    <row r="189" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A189" s="19">
         <v>44427</v>
       </c>
@@ -12032,7 +12037,7 @@
         <v>583.33333333333337</v>
       </c>
     </row>
-    <row r="190" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A190" s="19">
         <v>44427</v>
       </c>
@@ -12091,7 +12096,7 @@
         <v>37.916666666666671</v>
       </c>
     </row>
-    <row r="191" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A191" s="19">
         <v>44427</v>
       </c>
@@ -12153,7 +12158,7 @@
         <v>39.861111111111107</v>
       </c>
     </row>
-    <row r="192" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A192" s="19">
         <v>44427</v>
       </c>
@@ -12215,7 +12220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A193" s="19">
         <v>44427</v>
       </c>
@@ -12277,15 +12282,15 @@
         <v>23.333333333333332</v>
       </c>
     </row>
-    <row r="194" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A194" s="19">
         <v>44427</v>
       </c>
       <c r="B194">
         <v>1021060080</v>
       </c>
-      <c r="C194" t="s">
-        <v>87</v>
+      <c r="C194">
+        <v>18</v>
       </c>
       <c r="D194" t="s">
         <v>29</v>
@@ -12324,7 +12329,7 @@
         <v>647.5</v>
       </c>
     </row>
-    <row r="195" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A195" s="19">
         <v>44427</v>
       </c>
@@ -12371,7 +12376,7 @@
         <v>672.77777777777783</v>
       </c>
     </row>
-    <row r="196" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A196" s="19">
         <v>44428</v>
       </c>
@@ -12433,7 +12438,7 @@
         <v>27.222222222222221</v>
       </c>
     </row>
-    <row r="197" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A197" s="19">
         <v>44428</v>
       </c>
@@ -12456,7 +12461,7 @@
         <v>44428.416666666664</v>
       </c>
       <c r="H197" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I197" s="20">
         <v>44428.436111111114</v>
@@ -12495,7 +12500,7 @@
         <v>36.944444444444443</v>
       </c>
     </row>
-    <row r="198" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A198" s="19">
         <v>44428</v>
       </c>
@@ -12557,7 +12562,7 @@
         <v>26.25</v>
       </c>
     </row>
-    <row r="199" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A199" s="19">
         <v>44428</v>
       </c>
@@ -12619,7 +12624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A200" s="19">
         <v>44428</v>
       </c>
@@ -12681,7 +12686,7 @@
         <v>40.833333333333329</v>
       </c>
     </row>
-    <row r="201" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A201" s="19">
         <v>44428</v>
       </c>
@@ -12743,7 +12748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A202" s="19">
         <v>44428</v>
       </c>
@@ -12796,7 +12801,7 @@
         <v>642.63888888888891</v>
       </c>
     </row>
-    <row r="203" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A203" s="19">
         <v>44428</v>
       </c>
@@ -12858,15 +12863,15 @@
         <v>112.77777777777779</v>
       </c>
     </row>
-    <row r="204" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A204" s="19">
         <v>44428</v>
       </c>
       <c r="B204">
         <v>1021060049</v>
       </c>
-      <c r="C204" t="s">
-        <v>89</v>
+      <c r="C204">
+        <v>3</v>
       </c>
       <c r="D204" t="s">
         <v>26</v>
@@ -12920,7 +12925,7 @@
         <v>77.777777777777771</v>
       </c>
     </row>
-    <row r="205" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A205" s="19">
         <v>44428</v>
       </c>
@@ -12985,7 +12990,7 @@
         <v>24.305555555555557</v>
       </c>
     </row>
-    <row r="206" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A206" s="19">
         <v>44428</v>
       </c>
@@ -13008,7 +13013,7 @@
         <v>44428.68472222222</v>
       </c>
       <c r="H206" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I206" s="20">
         <v>44428.6875</v>
@@ -13047,7 +13052,7 @@
         <v>19.444444444444443</v>
       </c>
     </row>
-    <row r="207" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A207" s="19">
         <v>44429</v>
       </c>
@@ -13094,7 +13099,7 @@
         <v>515.27777777777783</v>
       </c>
     </row>
-    <row r="208" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A208" s="19">
         <v>44429</v>
       </c>
@@ -13156,7 +13161,7 @@
         <v>22.361111111111114</v>
       </c>
     </row>
-    <row r="209" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A209" s="19">
         <v>44429</v>
       </c>
@@ -13215,7 +13220,7 @@
         <v>37.916666666666671</v>
       </c>
     </row>
-    <row r="210" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A210" s="19">
         <v>44429</v>
       </c>
@@ -13277,7 +13282,7 @@
         <v>20.416666666666664</v>
       </c>
     </row>
-    <row r="211" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A211" s="19">
         <v>44429</v>
       </c>
@@ -13330,7 +13335,7 @@
         <v>560.97222222222229</v>
       </c>
     </row>
-    <row r="212" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A212" s="19">
         <v>44429</v>
       </c>
@@ -13392,7 +13397,7 @@
         <v>70.972222222222229</v>
       </c>
     </row>
-    <row r="213" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A213" s="19">
         <v>44429</v>
       </c>
@@ -13454,7 +13459,7 @@
         <v>16.527777777777779</v>
       </c>
     </row>
-    <row r="214" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A214" s="19">
         <v>44429</v>
       </c>
@@ -13516,7 +13521,7 @@
         <v>54.444444444444443</v>
       </c>
     </row>
-    <row r="215" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A215" s="19">
         <v>44429</v>
       </c>
@@ -13578,7 +13583,7 @@
         <v>58.333333333333329</v>
       </c>
     </row>
-    <row r="216" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A216" s="19">
         <v>44429</v>
       </c>
@@ -13640,7 +13645,7 @@
         <v>63.194444444444443</v>
       </c>
     </row>
-    <row r="217" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A217" s="19">
         <v>44429</v>
       </c>
@@ -13693,7 +13698,7 @@
         <v>656.25</v>
       </c>
     </row>
-    <row r="218" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A218" s="19">
         <v>44429</v>
       </c>
@@ -13746,7 +13751,7 @@
         <v>670.83333333333337</v>
       </c>
     </row>
-    <row r="219" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A219" s="19">
         <v>44429</v>
       </c>
@@ -13793,7 +13798,7 @@
         <v>693.19444444444434</v>
       </c>
     </row>
-    <row r="220" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A220" s="19">
         <v>44430</v>
       </c>
@@ -13825,7 +13830,7 @@
         <v>44430.427777777775</v>
       </c>
       <c r="K220" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="N220" s="16">
         <v>3.4722222222222224E-2</v>
@@ -13855,7 +13860,7 @@
         <v>48.611111111111114</v>
       </c>
     </row>
-    <row r="221" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A221" s="19">
         <v>44430</v>
       </c>
@@ -13887,7 +13892,7 @@
         <v>44430.463194444441</v>
       </c>
       <c r="K221" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="N221" s="16">
         <v>6.458333333333334E-2</v>
@@ -13917,7 +13922,7 @@
         <v>90.416666666666671</v>
       </c>
     </row>
-    <row r="222" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A222" s="19">
         <v>44430</v>
       </c>
@@ -13964,7 +13969,7 @@
         <v>645.55555555555554</v>
       </c>
     </row>
-    <row r="223" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A223" s="19">
         <v>44430</v>
       </c>
@@ -13987,7 +13992,7 @@
         <v>44430.469444444447</v>
       </c>
       <c r="H223" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I223" s="20">
         <v>44430.513888888891</v>
@@ -14026,7 +14031,7 @@
         <v>72.916666666666671</v>
       </c>
     </row>
-    <row r="224" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A224" s="19">
         <v>44431</v>
       </c>
@@ -14061,7 +14066,7 @@
         <v>38</v>
       </c>
       <c r="L224" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="N224" s="16">
         <v>7.4305555555555555E-2</v>
@@ -14091,7 +14096,7 @@
         <v>104.02777777777777</v>
       </c>
     </row>
-    <row r="225" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A225" s="19">
         <v>44431</v>
       </c>
@@ -14153,7 +14158,7 @@
         <v>45.69444444444445</v>
       </c>
     </row>
-    <row r="226" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A226" s="19">
         <v>44431</v>
       </c>
@@ -14200,7 +14205,7 @@
         <v>535.69444444444446</v>
       </c>
     </row>
-    <row r="227" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A227" s="19">
         <v>44431</v>
       </c>
@@ -14265,7 +14270,7 @@
         <v>22.361111111111114</v>
       </c>
     </row>
-    <row r="228" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A228" s="19">
         <v>44431</v>
       </c>
@@ -14327,7 +14332,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="229" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A229" s="19">
         <v>44431</v>
       </c>
@@ -14383,7 +14388,7 @@
         <v>30.138888888888893</v>
       </c>
     </row>
-    <row r="230" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A230" s="19">
         <v>44431</v>
       </c>
@@ -14445,7 +14450,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="231" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A231" s="19">
         <v>44431</v>
       </c>
@@ -14507,7 +14512,7 @@
         <v>38.888888888888886</v>
       </c>
     </row>
-    <row r="232" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A232" s="19">
         <v>44431</v>
       </c>
@@ -14551,7 +14556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A233" s="19">
         <v>44431</v>
       </c>
@@ -14613,7 +14618,7 @@
         <v>37.916666666666671</v>
       </c>
     </row>
-    <row r="234" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A234" s="19">
         <v>44431</v>
       </c>
@@ -14660,7 +14665,7 @@
         <v>814.72222222222229</v>
       </c>
     </row>
-    <row r="235" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A235" s="19">
         <v>44431</v>
       </c>
@@ -14707,7 +14712,7 @@
         <v>826.38888888888891</v>
       </c>
     </row>
-    <row r="236" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A236" s="19">
         <v>44431</v>
       </c>
@@ -14769,7 +14774,7 @@
         <v>29.166666666666664</v>
       </c>
     </row>
-    <row r="237" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A237" s="19">
         <v>44431</v>
       </c>
@@ -14816,7 +14821,7 @@
         <v>923.61111111111109</v>
       </c>
     </row>
-    <row r="238" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A238" s="19">
         <v>44431</v>
       </c>
@@ -14845,7 +14850,7 @@
         <v>44431.604166666664</v>
       </c>
       <c r="K238" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L238" t="s">
         <v>47</v>
@@ -14878,7 +14883,7 @@
         <v>24.305555555555557</v>
       </c>
     </row>
-    <row r="239" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A239" s="19">
         <v>44431</v>
       </c>
@@ -14940,7 +14945,7 @@
         <v>35.972222222222229</v>
       </c>
     </row>
-    <row r="240" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A240" s="19">
         <v>44432</v>
       </c>
@@ -15002,7 +15007,7 @@
         <v>76.805555555555557</v>
       </c>
     </row>
-    <row r="241" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A241" s="19">
         <v>44432</v>
       </c>
@@ -15064,7 +15069,7 @@
         <v>32.083333333333336</v>
       </c>
     </row>
-    <row r="242" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A242" s="19">
         <v>44432</v>
       </c>
@@ -15123,7 +15128,7 @@
         <v>49.583333333333329</v>
       </c>
     </row>
-    <row r="243" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A243" s="19">
         <v>44432</v>
       </c>
@@ -15176,7 +15181,7 @@
         <v>577.5</v>
       </c>
     </row>
-    <row r="244" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A244" s="19">
         <v>44432</v>
       </c>
@@ -15208,7 +15213,7 @@
         <v>44432.475694444445</v>
       </c>
       <c r="K244" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="N244" s="16">
         <v>5.4166666666666669E-2</v>
@@ -15238,7 +15243,7 @@
         <v>75.833333333333343</v>
       </c>
     </row>
-    <row r="245" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A245" s="19">
         <v>44432</v>
       </c>
@@ -15300,7 +15305,7 @@
         <v>72.916666666666671</v>
       </c>
     </row>
-    <row r="246" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A246" s="19">
         <v>44432</v>
       </c>
@@ -15323,7 +15328,7 @@
         <v>44432.443055555559</v>
       </c>
       <c r="H246" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I246" s="20">
         <v>44432.45416666667</v>
@@ -15362,7 +15367,7 @@
         <v>23.333333333333332</v>
       </c>
     </row>
-    <row r="247" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A247" s="19">
         <v>44432</v>
       </c>
@@ -15424,7 +15429,7 @@
         <v>7.7777777777777777</v>
       </c>
     </row>
-    <row r="248" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A248" s="19">
         <v>44432</v>
       </c>
@@ -15486,7 +15491,7 @@
         <v>19.444444444444443</v>
       </c>
     </row>
-    <row r="249" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A249" s="19">
         <v>44432</v>
       </c>
@@ -15542,7 +15547,7 @@
         <v>21.388888888888889</v>
       </c>
     </row>
-    <row r="250" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A250" s="19">
         <v>44432</v>
       </c>
@@ -15604,7 +15609,7 @@
         <v>6.8055555555555554</v>
       </c>
     </row>
-    <row r="251" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A251" s="19">
         <v>44433</v>
       </c>
@@ -15666,7 +15671,7 @@
         <v>29.166666666666664</v>
       </c>
     </row>
-    <row r="252" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A252" s="19">
         <v>44433</v>
       </c>
@@ -15728,7 +15733,7 @@
         <v>25.277777777777779</v>
       </c>
     </row>
-    <row r="253" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A253" s="19">
         <v>44433</v>
       </c>
@@ -15790,7 +15795,7 @@
         <v>27.222222222222221</v>
       </c>
     </row>
-    <row r="254" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A254" s="19">
         <v>44433</v>
       </c>
@@ -15849,7 +15854,7 @@
         <v>34.027777777777779</v>
       </c>
     </row>
-    <row r="255" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A255" s="19">
         <v>44433</v>
       </c>
@@ -15881,7 +15886,7 @@
         <v>44433.459722222222</v>
       </c>
       <c r="K255" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L255" t="s">
         <v>30</v>
@@ -15914,7 +15919,7 @@
         <v>83.611111111111114</v>
       </c>
     </row>
-    <row r="256" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A256" s="19">
         <v>44433</v>
       </c>
@@ -15937,7 +15942,7 @@
         <v>44433.48333333333</v>
       </c>
       <c r="H256" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I256" s="20">
         <v>44433.489583333336</v>
@@ -15973,7 +15978,7 @@
         <v>119.58333333333331</v>
       </c>
     </row>
-    <row r="257" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A257" s="19">
         <v>44433</v>
       </c>
@@ -15996,7 +16001,7 @@
         <v>44433.444444444445</v>
       </c>
       <c r="H257" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I257" s="20">
         <v>44433.460416666669</v>
@@ -16035,7 +16040,7 @@
         <v>33.055555555555557</v>
       </c>
     </row>
-    <row r="258" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A258" s="19">
         <v>44433</v>
       </c>
@@ -16097,7 +16102,7 @@
         <v>28.194444444444446</v>
       </c>
     </row>
-    <row r="259" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A259" s="19">
         <v>44433</v>
       </c>
@@ -16129,7 +16134,7 @@
         <v>44433.500694444447</v>
       </c>
       <c r="K259" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="N259" s="16">
         <v>3.8194444444444441E-2</v>
@@ -16159,7 +16164,7 @@
         <v>53.472222222222214</v>
       </c>
     </row>
-    <row r="260" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A260" s="19">
         <v>44433</v>
       </c>
@@ -16215,7 +16220,7 @@
         <v>645.55555555555554</v>
       </c>
     </row>
-    <row r="261" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A261" s="19">
         <v>44433</v>
       </c>
@@ -16247,7 +16252,7 @@
         <v>44433.482638888891</v>
       </c>
       <c r="K261" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="N261" s="16">
         <v>6.9444444444444441E-3</v>
@@ -16277,7 +16282,7 @@
         <v>9.7222222222222214</v>
       </c>
     </row>
-    <row r="262" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A262" s="19">
         <v>44433</v>
       </c>
@@ -16300,7 +16305,7 @@
         <v>44433.54583333333</v>
       </c>
       <c r="H262" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I262" s="20">
         <v>44433.552083333336</v>
@@ -16339,7 +16344,7 @@
         <v>26.25</v>
       </c>
     </row>
-    <row r="263" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A263" s="19">
         <v>44433</v>
       </c>
@@ -16404,7 +16409,7 @@
         <v>32.083333333333336</v>
       </c>
     </row>
-    <row r="264" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A264" s="19">
         <v>44434</v>
       </c>
@@ -16460,7 +16465,7 @@
         <v>509.4444444444444</v>
       </c>
     </row>
-    <row r="265" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A265" s="19">
         <v>44434</v>
       </c>
@@ -16522,7 +16527,7 @@
         <v>25.277777777777779</v>
       </c>
     </row>
-    <row r="266" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A266" s="19">
         <v>44434</v>
       </c>
@@ -16575,7 +16580,7 @@
         <v>534.72222222222217</v>
       </c>
     </row>
-    <row r="267" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A267" s="19">
         <v>44434</v>
       </c>
@@ -16601,7 +16606,7 @@
         <v>44434.420138888891</v>
       </c>
       <c r="K267" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="N267" s="16">
         <v>2.2916666666666669E-2</v>
@@ -16631,7 +16636,7 @@
         <v>32.083333333333336</v>
       </c>
     </row>
-    <row r="268" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A268" s="19">
         <v>44434</v>
       </c>
@@ -16693,7 +16698,7 @@
         <v>23.333333333333332</v>
       </c>
     </row>
-    <row r="269" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A269" s="19">
         <v>44434</v>
       </c>
@@ -16755,7 +16760,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="270" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A270" s="19">
         <v>44434</v>
       </c>
@@ -16802,7 +16807,7 @@
         <v>591.11111111111109</v>
       </c>
     </row>
-    <row r="271" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A271" s="19">
         <v>44434</v>
       </c>
@@ -16855,7 +16860,7 @@
         <v>631.94444444444446</v>
       </c>
     </row>
-    <row r="272" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A272" s="19">
         <v>44434</v>
       </c>
@@ -16917,7 +16922,7 @@
         <v>26.25</v>
       </c>
     </row>
-    <row r="273" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A273" s="19">
         <v>44434</v>
       </c>
@@ -16979,7 +16984,7 @@
         <v>62.222222222222221</v>
       </c>
     </row>
-    <row r="274" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A274" s="19">
         <v>44435</v>
       </c>
@@ -17032,7 +17037,7 @@
         <v>496.8055555555556</v>
       </c>
     </row>
-    <row r="275" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A275" s="19">
         <v>44435</v>
       </c>
@@ -17082,7 +17087,7 @@
         <v>520.1388888888888</v>
       </c>
     </row>
-    <row r="276" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A276" s="19">
         <v>44435</v>
       </c>
@@ -17144,7 +17149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A277" s="19">
         <v>44435</v>
       </c>
@@ -17167,7 +17172,7 @@
         <v>44435.378472222219</v>
       </c>
       <c r="H277" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I277" s="20">
         <v>44435.397222222222</v>
@@ -17203,7 +17208,7 @@
         <v>34.027777777777779</v>
       </c>
     </row>
-    <row r="278" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A278" s="19">
         <v>44435</v>
       </c>
@@ -17226,10 +17231,10 @@
         <v>44435.377083333333</v>
       </c>
       <c r="H278" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K278" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="N278" s="16">
         <v>0.3743055555555555</v>
@@ -17259,7 +17264,7 @@
         <v>524.02777777777771</v>
       </c>
     </row>
-    <row r="279" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A279" s="19">
         <v>44435</v>
       </c>
@@ -17282,7 +17287,7 @@
         <v>44435.384027777778</v>
       </c>
       <c r="H279" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I279" s="20">
         <v>44435.397916666669</v>
@@ -17318,7 +17323,7 @@
         <v>22.361111111111114</v>
       </c>
     </row>
-    <row r="280" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A280" s="19">
         <v>44435</v>
       </c>
@@ -17341,7 +17346,7 @@
         <v>44435.394444444442</v>
       </c>
       <c r="H280" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I280" s="20">
         <v>44435.411111111112</v>
@@ -17377,7 +17382,7 @@
         <v>29.166666666666664</v>
       </c>
     </row>
-    <row r="281" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A281" s="19">
         <v>44435</v>
       </c>
@@ -17400,7 +17405,7 @@
         <v>44435.411111111112</v>
       </c>
       <c r="H281" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I281" s="20">
         <v>44435.420138888891</v>
@@ -17439,7 +17444,7 @@
         <v>21.388888888888889</v>
       </c>
     </row>
-    <row r="282" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A282" s="19">
         <v>44435</v>
       </c>
@@ -17462,7 +17467,7 @@
         <v>44435.4375</v>
       </c>
       <c r="H282" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I282" s="20">
         <v>44435.45208333333</v>
@@ -17501,7 +17506,7 @@
         <v>26.25</v>
       </c>
     </row>
-    <row r="283" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A283" s="19">
         <v>44435</v>
       </c>
@@ -17524,7 +17529,7 @@
         <v>44435.486805555556</v>
       </c>
       <c r="H283" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I283" s="20">
         <v>44435.470833333333</v>
@@ -17566,7 +17571,7 @@
         <v>43.75</v>
       </c>
     </row>
-    <row r="284" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A284" s="19">
         <v>44435</v>
       </c>
@@ -17628,7 +17633,7 @@
         <v>49.583333333333329</v>
       </c>
     </row>
-    <row r="285" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A285" s="19">
         <v>44435</v>
       </c>
@@ -17651,7 +17656,7 @@
         <v>44435.461111111108</v>
       </c>
       <c r="H285" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I285" s="20">
         <v>44435.472222222219</v>
@@ -17690,7 +17695,7 @@
         <v>50.555555555555557</v>
       </c>
     </row>
-    <row r="286" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A286" s="19">
         <v>44435</v>
       </c>
@@ -17752,7 +17757,7 @@
         <v>50.555555555555557</v>
       </c>
     </row>
-    <row r="287" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A287" s="19">
         <v>44435</v>
       </c>
@@ -17814,7 +17819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A288" s="19">
         <v>44435</v>
       </c>
@@ -17876,7 +17881,7 @@
         <v>21.388888888888889</v>
       </c>
     </row>
-    <row r="289" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A289" s="19">
         <v>44435</v>
       </c>
@@ -17938,7 +17943,7 @@
         <v>28.194444444444446</v>
       </c>
     </row>
-    <row r="290" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A290" s="19">
         <v>44435</v>
       </c>
@@ -17991,7 +17996,7 @@
         <v>949.8611111111112</v>
       </c>
     </row>
-    <row r="291" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A291" s="19">
         <v>44435</v>
       </c>
@@ -18053,7 +18058,7 @@
         <v>42.777777777777779</v>
       </c>
     </row>
-    <row r="292" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A292" s="19">
         <v>44436</v>
       </c>
@@ -18118,7 +18123,7 @@
         <v>63.194444444444443</v>
       </c>
     </row>
-    <row r="293" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A293" s="19">
         <v>44436</v>
       </c>
@@ -18141,7 +18146,7 @@
         <v>44436.370833333334</v>
       </c>
       <c r="H293" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I293" s="20">
         <v>44436.388194444444</v>
@@ -18180,7 +18185,7 @@
         <v>34.027777777777779</v>
       </c>
     </row>
-    <row r="294" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A294" s="19">
         <v>44436</v>
       </c>
@@ -18242,7 +18247,7 @@
         <v>24.305555555555557</v>
       </c>
     </row>
-    <row r="295" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A295" s="19">
         <v>44436</v>
       </c>
@@ -18307,7 +18312,7 @@
         <v>61.250000000000007</v>
       </c>
     </row>
-    <row r="296" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A296" s="19">
         <v>44436</v>
       </c>
@@ -18369,7 +18374,7 @@
         <v>37.916666666666671</v>
       </c>
     </row>
-    <row r="297" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A297" s="19">
         <v>44436</v>
       </c>
@@ -18431,7 +18436,7 @@
         <v>13.611111111111111</v>
       </c>
     </row>
-    <row r="298" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A298" s="19">
         <v>44436</v>
       </c>
@@ -18493,7 +18498,7 @@
         <v>21.388888888888889</v>
       </c>
     </row>
-    <row r="299" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A299" s="19">
         <v>44436</v>
       </c>
@@ -18555,7 +18560,7 @@
         <v>38.888888888888886</v>
       </c>
     </row>
-    <row r="300" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A300" s="19">
         <v>44436</v>
       </c>
@@ -18617,7 +18622,7 @@
         <v>33.055555555555557</v>
       </c>
     </row>
-    <row r="301" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A301" s="19">
         <v>44436</v>
       </c>
@@ -18679,7 +18684,7 @@
         <v>30.138888888888893</v>
       </c>
     </row>
-    <row r="302" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A302" s="19">
         <v>44436</v>
       </c>
@@ -18744,7 +18749,7 @@
         <v>63.194444444444443</v>
       </c>
     </row>
-    <row r="303" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A303" s="19">
         <v>44436</v>
       </c>
@@ -18806,7 +18811,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="304" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A304" s="19">
         <v>44436</v>
       </c>
@@ -18871,7 +18876,7 @@
         <v>12.638888888888889</v>
       </c>
     </row>
-    <row r="305" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A305" s="19">
         <v>44437</v>
       </c>
@@ -18933,7 +18938,7 @@
         <v>14.583333333333332</v>
       </c>
     </row>
-    <row r="306" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A306" s="19">
         <v>44437</v>
       </c>
@@ -18995,7 +19000,7 @@
         <v>20.416666666666664</v>
       </c>
     </row>
-    <row r="307" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A307" s="19">
         <v>44437</v>
       </c>
@@ -19057,7 +19062,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="308" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A308" s="19">
         <v>44437</v>
       </c>
@@ -19119,7 +19124,7 @@
         <v>34.027777777777779</v>
       </c>
     </row>
-    <row r="309" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A309" s="19">
         <v>44437</v>
       </c>
@@ -19181,7 +19186,7 @@
         <v>19.444444444444443</v>
       </c>
     </row>
-    <row r="310" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A310" s="19">
         <v>44437</v>
       </c>
@@ -19243,7 +19248,7 @@
         <v>15.555555555555555</v>
       </c>
     </row>
-    <row r="311" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A311" s="19">
         <v>44437</v>
       </c>
@@ -19305,7 +19310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A312" s="19">
         <v>44437</v>
       </c>
@@ -19328,7 +19333,7 @@
         <v>44437.512499999997</v>
       </c>
       <c r="H312" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I312" s="20">
         <v>44437.533333333333</v>
@@ -19367,7 +19372,7 @@
         <v>29.166666666666664</v>
       </c>
     </row>
-    <row r="313" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A313" s="19">
         <v>44438</v>
       </c>
@@ -19426,7 +19431,7 @@
         <v>34.027777777777779</v>
       </c>
     </row>
-    <row r="314" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A314" s="19">
         <v>44438</v>
       </c>
@@ -19488,7 +19493,7 @@
         <v>4.8611111111111107</v>
       </c>
     </row>
-    <row r="315" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A315" s="19">
         <v>44438</v>
       </c>
@@ -19553,7 +19558,7 @@
         <v>60.277777777777786</v>
       </c>
     </row>
-    <row r="316" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A316" s="19">
         <v>44438</v>
       </c>
@@ -19618,7 +19623,7 @@
         <v>34.027777777777779</v>
       </c>
     </row>
-    <row r="317" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A317" s="19">
         <v>44438</v>
       </c>
@@ -19683,7 +19688,7 @@
         <v>38.888888888888886</v>
       </c>
     </row>
-    <row r="318" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A318" s="19">
         <v>44438</v>
       </c>
@@ -19742,7 +19747,7 @@
         <v>24.305555555555557</v>
       </c>
     </row>
-    <row r="319" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A319" s="19">
         <v>44438</v>
       </c>
@@ -19807,7 +19812,7 @@
         <v>10.694444444444445</v>
       </c>
     </row>
-    <row r="320" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A320" s="19">
         <v>44438</v>
       </c>
@@ -19869,7 +19874,7 @@
         <v>102.08333333333334</v>
       </c>
     </row>
-    <row r="321" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A321" s="19">
         <v>44438</v>
       </c>
@@ -19931,7 +19936,7 @@
         <v>6.8055555555555554</v>
       </c>
     </row>
-    <row r="322" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A322" s="19">
         <v>44438</v>
       </c>
@@ -19993,7 +19998,7 @@
         <v>9.7222222222222214</v>
       </c>
     </row>
-    <row r="323" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A323" s="19">
         <v>44438</v>
       </c>
@@ -20055,7 +20060,7 @@
         <v>68.055555555555557</v>
       </c>
     </row>
-    <row r="324" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A324" s="19">
         <v>44438</v>
       </c>
@@ -20117,7 +20122,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="325" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A325" s="19">
         <v>44438</v>
       </c>
@@ -20164,7 +20169,7 @@
         <v>1023.7500000000001</v>
       </c>
     </row>
-    <row r="326" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A326" s="19">
         <v>44439</v>
       </c>
@@ -20226,7 +20231,7 @@
         <v>54.444444444444443</v>
       </c>
     </row>
-    <row r="327" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A327" s="19">
         <v>44439</v>
       </c>
@@ -20249,7 +20254,7 @@
         <v>44439.378472222219</v>
       </c>
       <c r="H327" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I327" s="20">
         <v>44439.394444444442</v>
@@ -20288,7 +20293,7 @@
         <v>30.138888888888893</v>
       </c>
     </row>
-    <row r="328" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A328" s="19">
         <v>44439</v>
       </c>
@@ -20350,7 +20355,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="329" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A329" s="19">
         <v>44439</v>
       </c>
@@ -20412,7 +20417,7 @@
         <v>18.472222222222221</v>
       </c>
     </row>
-    <row r="330" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A330" s="19">
         <v>44439</v>
       </c>
@@ -20474,7 +20479,7 @@
         <v>66.111111111111114</v>
       </c>
     </row>
-    <row r="331" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A331" s="19">
         <v>44439</v>
       </c>
@@ -20536,7 +20541,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="332" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A332" s="19">
         <v>44439</v>
       </c>
@@ -20595,7 +20600,7 @@
         <v>18.472222222222221</v>
       </c>
     </row>
-    <row r="333" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A333" s="19">
         <v>44439</v>
       </c>
@@ -20657,7 +20662,7 @@
         <v>93.333333333333329</v>
       </c>
     </row>
-    <row r="334" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A334" s="19">
         <v>44439</v>
       </c>
@@ -20722,7 +20727,7 @@
         <v>61.250000000000007</v>
       </c>
     </row>
-    <row r="335" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A335" s="19">
         <v>44439</v>
       </c>
@@ -20784,7 +20789,7 @@
         <v>16.527777777777779</v>
       </c>
     </row>
-    <row r="336" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A336" s="19">
         <v>44439</v>
       </c>
@@ -20846,7 +20851,7 @@
         <v>91.3888888888889</v>
       </c>
     </row>
-    <row r="337" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A337" s="19">
         <v>44439</v>
       </c>
@@ -20908,7 +20913,7 @@
         <v>35.972222222222229</v>
       </c>
     </row>
-    <row r="338" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A338" s="19">
         <v>44439</v>
       </c>
@@ -20970,7 +20975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="339" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A339" s="19">
         <v>44439</v>
       </c>
@@ -21032,7 +21037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="340" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A340" s="19">
         <v>44439</v>
       </c>
@@ -21094,7 +21099,7 @@
         <v>9.7222222222222214</v>
       </c>
     </row>
-    <row r="341" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A341" s="19">
         <v>44439</v>
       </c>
@@ -21156,7 +21161,7 @@
         <v>16.527777777777779</v>
       </c>
     </row>
-    <row r="342" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A342" s="19">
         <v>44439</v>
       </c>
@@ -21218,7 +21223,7 @@
         <v>320.83333333333331</v>
       </c>
     </row>
-    <row r="343" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A343" s="19">
         <v>44439</v>
       </c>
@@ -21280,7 +21285,7 @@
         <v>30.138888888888893</v>
       </c>
     </row>
-    <row r="344" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A344" s="19">
         <v>44439</v>
       </c>
@@ -21342,7 +21347,7 @@
         <v>14.583333333333332</v>
       </c>
     </row>
-    <row r="345" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A345" s="19">
         <v>44439</v>
       </c>
@@ -21401,7 +21406,7 @@
         <v>18.472222222222221</v>
       </c>
     </row>
-    <row r="346" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A346" s="1"/>
       <c r="B346" s="2"/>
       <c r="C346" s="3"/>
@@ -21432,7 +21437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="347" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A347" s="8"/>
       <c r="B347" s="9"/>
       <c r="C347" s="10"/>
@@ -21463,7 +21468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="348" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A348" s="1"/>
       <c r="B348" s="2"/>
       <c r="C348" s="3"/>
@@ -21494,7 +21499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="349" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A349" s="8"/>
       <c r="B349" s="9"/>
       <c r="C349" s="10"/>
@@ -21525,7 +21530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="350" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A350" s="1"/>
       <c r="B350" s="2"/>
       <c r="C350" s="3"/>
@@ -21556,7 +21561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="351" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A351" s="8"/>
       <c r="B351" s="9"/>
       <c r="C351" s="10"/>
@@ -21587,7 +21592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="352" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A352" s="1"/>
       <c r="B352" s="2"/>
       <c r="C352" s="3"/>
@@ -21618,7 +21623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="353" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A353" s="8"/>
       <c r="B353" s="9"/>
       <c r="C353" s="10"/>
@@ -21649,7 +21654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="354" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A354" s="1"/>
       <c r="B354" s="2"/>
       <c r="C354" s="3"/>
@@ -21680,7 +21685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="355" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A355" s="8"/>
       <c r="B355" s="9"/>
       <c r="C355" s="10"/>
@@ -21711,7 +21716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="356" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A356" s="1"/>
       <c r="B356" s="2"/>
       <c r="C356" s="3"/>
@@ -21742,7 +21747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="357" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A357" s="8"/>
       <c r="B357" s="9"/>
       <c r="C357" s="10"/>
@@ -21773,7 +21778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="358" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A358" s="1"/>
       <c r="B358" s="2"/>
       <c r="C358" s="3"/>
@@ -21804,7 +21809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="359" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A359" s="8"/>
       <c r="B359" s="9"/>
       <c r="C359" s="10"/>
@@ -21835,7 +21840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="360" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A360" s="1"/>
       <c r="B360" s="2"/>
       <c r="C360" s="3"/>
@@ -21866,7 +21871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="361" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A361" s="8"/>
       <c r="B361" s="9"/>
       <c r="C361" s="10"/>
@@ -21897,7 +21902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A362" s="1"/>
       <c r="B362" s="2"/>
       <c r="C362" s="3"/>
@@ -21928,7 +21933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="363" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A363" s="8"/>
       <c r="B363" s="9"/>
       <c r="C363" s="10"/>
@@ -21959,7 +21964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="364" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A364" s="1"/>
       <c r="B364" s="2"/>
       <c r="C364" s="3"/>
@@ -21990,7 +21995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="365" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A365" s="8"/>
       <c r="B365" s="9"/>
       <c r="C365" s="10"/>
@@ -22021,7 +22026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="366" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A366" s="1"/>
       <c r="B366" s="2"/>
       <c r="C366" s="3"/>
@@ -22052,7 +22057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="367" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A367" s="8"/>
       <c r="B367" s="9"/>
       <c r="C367" s="10"/>
@@ -22083,7 +22088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="368" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A368" s="1"/>
       <c r="B368" s="2"/>
       <c r="C368" s="3"/>
@@ -22114,7 +22119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="369" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A369" s="8"/>
       <c r="B369" s="9"/>
       <c r="C369" s="10"/>
@@ -22145,7 +22150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="370" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A370" s="1"/>
       <c r="B370" s="2"/>
       <c r="C370" s="3"/>
@@ -22176,7 +22181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="371" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A371" s="8"/>
       <c r="B371" s="9"/>
       <c r="C371" s="10"/>
@@ -22207,7 +22212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="372" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A372" s="1"/>
       <c r="B372" s="2"/>
       <c r="C372" s="3"/>
@@ -22238,7 +22243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="373" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A373" s="8"/>
       <c r="B373" s="9"/>
       <c r="C373" s="10"/>
@@ -22269,7 +22274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="374" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A374" s="1"/>
       <c r="B374" s="2"/>
       <c r="C374" s="3"/>
@@ -22300,7 +22305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="375" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A375" s="8"/>
       <c r="B375" s="9"/>
       <c r="C375" s="10"/>
@@ -22331,7 +22336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="376" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A376" s="1"/>
       <c r="B376" s="2"/>
       <c r="C376" s="3"/>
@@ -22362,7 +22367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="377" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A377" s="8"/>
       <c r="B377" s="9"/>
       <c r="C377" s="10"/>
@@ -22393,7 +22398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="378" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A378" s="1"/>
       <c r="B378" s="2"/>
       <c r="C378" s="3"/>
@@ -22424,7 +22429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="379" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A379" s="8"/>
       <c r="B379" s="9"/>
       <c r="C379" s="10"/>
@@ -22455,7 +22460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="380" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A380" s="1"/>
       <c r="B380" s="2"/>
       <c r="C380" s="3"/>
@@ -22486,7 +22491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="381" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A381" s="8"/>
       <c r="B381" s="9"/>
       <c r="C381" s="10"/>
@@ -22517,7 +22522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="382" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="382" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A382" s="1"/>
       <c r="B382" s="2"/>
       <c r="C382" s="3"/>
@@ -22548,7 +22553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="383" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="383" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A383" s="8"/>
       <c r="B383" s="9"/>
       <c r="C383" s="10"/>
@@ -22579,7 +22584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="384" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="384" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A384" s="1"/>
       <c r="B384" s="2"/>
       <c r="C384" s="3"/>
@@ -22610,7 +22615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="385" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="385" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A385" s="8"/>
       <c r="B385" s="9"/>
       <c r="C385" s="10"/>
@@ -22641,7 +22646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="386" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="386" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A386" s="1"/>
       <c r="B386" s="2"/>
       <c r="C386" s="3"/>
@@ -22672,7 +22677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="387" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="387" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A387" s="8"/>
       <c r="B387" s="9"/>
       <c r="C387" s="10"/>
@@ -22703,7 +22708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="388" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="388" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A388" s="1"/>
       <c r="B388" s="2"/>
       <c r="C388" s="3"/>
@@ -22734,7 +22739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="389" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="389" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A389" s="8"/>
       <c r="B389" s="9"/>
       <c r="C389" s="10"/>
@@ -22765,7 +22770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="390" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="390" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A390" s="1"/>
       <c r="B390" s="2"/>
       <c r="C390" s="3"/>
@@ -22797,6 +22802,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:W345" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>